<commit_message>
Added a Query to check inovice mops
</commit_message>
<xml_diff>
--- a/V3.1.0 - Table comparison.xlsx
+++ b/V3.1.0 - Table comparison.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5764B31-029E-4407-AB97-B5012C1FDE92}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{833DDCCA-E4D3-4886-9826-DD1B07C9D100}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="51">
   <si>
     <t>tbl_accessories</t>
   </si>
@@ -158,13 +158,91 @@
   </si>
   <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t>Tbl_invoiceItem</t>
+  </si>
+  <si>
+    <t>Tbl_invoiceItemREturns</t>
+  </si>
+  <si>
+    <r>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">          </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Description</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">          </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TypeID</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">          </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Trade-in true or false</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -179,6 +257,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -313,7 +397,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -331,6 +415,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="8"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -611,10 +701,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:AF27"/>
+  <dimension ref="A2:AF34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1625,6 +1715,31 @@
         <v>45</v>
       </c>
     </row>
+    <row r="30" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A30" s="17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A31" s="17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A32" s="18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="18" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="18" t="s">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>